<commit_message>
actualizacion 16 de abril
</commit_message>
<xml_diff>
--- a/Resultados Experimentales/Headspace/Moldeo y Headspace Peliculas.xlsx
+++ b/Resultados Experimentales/Headspace/Moldeo y Headspace Peliculas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniandes-my.sharepoint.com/personal/df_rozo11_uniandes_edu_co/Documents/Duodecimo semestre/Repositorio_Maestria/Resultados Experimentales/Headspace/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CA077425-8C78-4BCD-8AE4-19824D536F75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{CA077425-8C78-4BCD-8AE4-19824D536F75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{772D8983-C92C-4EAE-A8CB-6602EBF6A098}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{FD01FDAC-61FF-4472-916D-FD331975B4C6}"/>
   </bookViews>
@@ -167,13 +167,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -494,249 +494,249 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F23484BD-2FA4-488F-A48E-08A7922AB26B}">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.86328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.19921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="2"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A2" s="3" t="s">
+      <c r="B1" s="5"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="2">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <f>B3*B2</f>
         <v>112</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="2"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A7" s="3" t="s">
+      <c r="B6" s="5"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="4">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="2">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="4">
         <f>B8*B7</f>
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="4">
         <f>B10/2</f>
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="4">
         <f>B11*12</f>
         <v>216</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A13" s="3" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A15" s="2" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A16" s="5" t="s">
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A17" s="3" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17" s="4">
         <v>9</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="4">
         <f>B17*4</f>
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A18" s="3" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B18" s="5">
+      <c r="B18" s="4">
         <f>36</f>
         <v>36</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18" s="4">
         <f t="shared" ref="C18:C19" si="0">B18*4</f>
         <v>144</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A19" s="3" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="5">
+      <c r="B19" s="4">
         <f>SUM(B17:B18)</f>
         <v>45</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C19" s="4">
         <f t="shared" si="0"/>
         <v>180</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A21" s="2" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A22" s="5" t="s">
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="5">
+      <c r="B22" s="4">
         <v>1</v>
       </c>
-      <c r="C22" s="5">
+      <c r="C22" s="4">
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A23" s="3" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B23" s="5">
+      <c r="B23" s="4">
         <v>30</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C23" s="4">
         <f>B23*C$22</f>
         <v>180</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A24" s="4" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B24" s="5">
+      <c r="B24" s="4">
         <v>10</v>
       </c>
-      <c r="C24" s="5">
+      <c r="C24" s="4">
         <f>B24*C$22</f>
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A25" s="4" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B25" s="5">
+      <c r="B25" s="4">
         <f>B24+B23</f>
         <v>40</v>
       </c>
-      <c r="C25" s="5">
+      <c r="C25" s="4">
         <f>C24+C23</f>
         <v>240</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A26" s="4" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B26" s="5">
+      <c r="B26" s="4">
         <f>INT(B25/12)</f>
         <v>3</v>
       </c>
-      <c r="C26" s="5">
+      <c r="C26" s="4">
         <f>INT(C25/12)</f>
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A27" s="4" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B27" s="5">
+      <c r="B27" s="4">
         <f>ROUNDUP(B24/$B$19,0)</f>
         <v>1</v>
       </c>
-      <c r="C27" s="5">
+      <c r="C27" s="4">
         <f>ROUNDUP(C24/$B$19,0)</f>
         <v>2</v>
       </c>
@@ -753,6 +753,90 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Is_Collaboration_Space_Locked xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
+    <Invited_Teachers xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
+    <IsNotebookLocked xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
+    <Teachers xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Teachers>
+    <Distribution_Groups xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
+    <Self_Registration_Enabled xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
+    <LMS_Mappings xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
+    <FolderType xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
+    <CultureName xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
+    <Templates xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
+    <Has_Teacher_Only_SectionGroup xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
+    <Members xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Members>
+    <Member_Groups xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Member_Groups>
+    <NotebookType xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
+    <Leaders xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Leaders>
+    <Has_Leaders_Only_SectionGroup xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
+    <Owner xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Owner>
+    <Math_Settings xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
+    <DefaultSectionNames xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
+    <Invited_Members xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
+    <AppVersion xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
+    <TeamsChannelId xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
+    <Invited_Students xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
+    <Invited_Leaders xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
+    <Students xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Students>
+    <Student_Groups xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Student_Groups>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101006E073622718B7D418B69CBE92FF13C49" ma:contentTypeVersion="39" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="e0b40c6a749bc4d602fb0fa807cb6535">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="2d185e16-06da-45ab-8500-654d664b7dd3" xmlns:ns4="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9f23f6d71d802450f7203042af7b69aa" ns3:_="" ns4:_="">
     <xsd:import namespace="2d185e16-06da-45ab-8500-654d664b7dd3"/>
@@ -1245,91 +1329,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{001AC61C-C96F-4D9B-9582-B5D1C1608E49}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Is_Collaboration_Space_Locked xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
-    <Invited_Teachers xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
-    <IsNotebookLocked xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
-    <Teachers xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Teachers>
-    <Distribution_Groups xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
-    <Self_Registration_Enabled xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
-    <LMS_Mappings xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
-    <FolderType xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
-    <CultureName xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
-    <Templates xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
-    <Has_Teacher_Only_SectionGroup xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
-    <Members xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Members>
-    <Member_Groups xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Member_Groups>
-    <NotebookType xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
-    <Leaders xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Leaders>
-    <Has_Leaders_Only_SectionGroup xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
-    <Owner xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Owner>
-    <Math_Settings xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
-    <DefaultSectionNames xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
-    <Invited_Members xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
-    <AppVersion xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
-    <TeamsChannelId xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
-    <Invited_Students xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
-    <Invited_Leaders xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc" xsi:nil="true"/>
-    <Students xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Students>
-    <Student_Groups xmlns="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Student_Groups>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2E5A63FC-38BB-41E2-B444-ED144048C3C2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96D52CFC-BBB9-4AE7-B297-765DEB67F8DA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1346,22 +1364,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2E5A63FC-38BB-41E2-B444-ED144048C3C2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{001AC61C-C96F-4D9B-9582-B5D1C1608E49}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="8f8a3fab-e0af-4131-8cc8-5f2165a4edfc"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>